<commit_message>
workinkg getting and passing data from .XLSX file to data provider
</commit_message>
<xml_diff>
--- a/dataSet.xlsx
+++ b/dataSet.xlsx
@@ -20,42 +20,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">name</t>
   </si>
   <si>
-    <t xml:space="preserve">roll</t>
-  </si>
-  <si>
-    <t xml:space="preserve">age</t>
-  </si>
-  <si>
-    <t xml:space="preserve">class</t>
-  </si>
-  <si>
-    <t xml:space="preserve">marks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">zipCode</t>
+    <t xml:space="preserve">emil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pass</t>
   </si>
   <si>
     <t xml:space="preserve">ajit</t>
   </si>
   <si>
-    <t xml:space="preserve">Eight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">roshan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">soy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ten</t>
+    <t xml:space="preserve">ajit@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123@ajit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ashishan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4146@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4146@yenzi</t>
   </si>
 </sst>
 </file>
@@ -65,7 +56,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -86,6 +77,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -130,12 +128,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -156,13 +158,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="181" zoomScaleNormal="181" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.73"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -174,77 +179,36 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="1" t="n">
-        <v>67</v>
-      </c>
-      <c r="F2" s="1" t="n">
-        <v>1001</v>
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="1" t="n">
-        <v>77</v>
-      </c>
-      <c r="F3" s="1" t="n">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="1" t="n">
-        <v>87</v>
-      </c>
-      <c r="F4" s="1" t="n">
-        <v>1003</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="ajit@gmail.com"/>
+    <hyperlink ref="C2" r:id="rId2" display="123@ajit"/>
+    <hyperlink ref="B3" r:id="rId3" display="4146@gmail.com"/>
+    <hyperlink ref="C3" r:id="rId4" display="4146@yenzi"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>